<commit_message>
Atualização das bases de dados, codigo e imagens
</commit_message>
<xml_diff>
--- a/dataset/corona_pred (1) old.xlsx
+++ b/dataset/corona_pred (1) old.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Octavio\Desktop\Projetos Python\Function Approximator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braeued1\Documents\Octavio\projetos\Covid19_data\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DBB643-3FA2-47B8-B53B-2C27F029FD93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="corona_pred (1)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>tempo</t>
   </si>
@@ -56,11 +57,14 @@
   <si>
     <t>Erro</t>
   </si>
+  <si>
+    <t>growth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,7 +498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -537,54 +541,57 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -600,9 +607,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -644,7 +651,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -670,7 +676,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1804,6 +1810,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E803-4CD8-8993-CD1FB9ECD229}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2929,6 +2940,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E803-4CD8-8993-CD1FB9ECD229}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4054,585 +4070,15 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Leitos</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'corona_pred (1)'!$G$2:$G$182</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="181"/>
-                <c:pt idx="0">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>55110</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E803-4CD8-8993-CD1FB9ECD229}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>Casos reais</c:v>
-          </c:tx>
+          <c:order val="3"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -4647,10 +4093,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'corona_pred (1)'!$H$2:$H$13</c:f>
+              <c:f>'corona_pred (1)'!$H$2:$H$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>151</c:v>
                 </c:pt>
@@ -4686,11 +4132,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2433</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3417</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3904</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4256</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4579</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E803-4CD8-8993-CD1FB9ECD229}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4745,7 +4214,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1592150752"/>
@@ -4803,7 +4272,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1592156736"/>
@@ -4820,7 +4289,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4846,7 +4314,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4876,7 +4344,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4888,9 +4356,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4927,7 +4395,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4953,7 +4420,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5643,690 +5110,15 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Leitos</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'corona_pred (1)'!$F$5:$F$37</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>43907</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43908</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43909</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43911</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43912</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43913</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43914</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43915</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43916</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43918</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43919</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43920</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43921</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43922</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43923</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43925</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43926</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43927</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43928</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43929</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43930</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43932</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>43934</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>43935</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43936</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>43937</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43939</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'corona_pred (1)'!$G$2:$G$182</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="181"/>
-                <c:pt idx="0">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>55110</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>55110</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-548A-463A-959A-5D275FB8069B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -6449,10 +5241,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'corona_pred (1)'!$H$2:$H$13</c:f>
+              <c:f>'corona_pred (1)'!$H$2:$H$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>151</c:v>
                 </c:pt>
@@ -6488,11 +5280,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2433</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2915</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3417</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3904</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4256</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4579</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-548A-463A-959A-5D275FB8069B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6547,7 +5362,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1724429296"/>
@@ -6605,7 +5420,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1724428752"/>
@@ -6622,7 +5437,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6648,7 +5462,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6678,12 +5492,305 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'corona_pred (1)'!$N$6:$N$19</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28260869565217389</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.30508474576271188</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19480519480519481</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2391304347826087</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19298245614035087</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16911764705882354</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26415094339622641</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD0E-4EF7-BB38-50C58BEB44B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="712298080"/>
+        <c:axId val="712304312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="712298080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712304312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="712304312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712298080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6730,6 +5837,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7801,24 +6948,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7835,20 +7504,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7860,6 +7535,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31C90D49-91F9-4B26-8DDB-8E9DDCD9A027}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8130,11 +7841,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N182"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8142,7 +7853,7 @@
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8177,10 +7888,13 @@
         <v>8</v>
       </c>
       <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8214,7 +7928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8247,7 +7961,7 @@
         <v>3</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K12" si="1">ABS(H3-D3)</f>
+        <f t="shared" ref="K3:K11" si="1">ABS(H3-D3)</f>
         <v>2.23552640786599</v>
       </c>
       <c r="L3">
@@ -8255,7 +7969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8284,7 +7998,7 @@
         <v>257</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J13" si="2">ABS(H4-I4)</f>
+        <f t="shared" ref="J4:J15" si="2">ABS(H4-I4)</f>
         <v>23</v>
       </c>
       <c r="K4">
@@ -8296,7 +8010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8339,12 +8053,12 @@
       <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f>ABS(L5-M5)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8387,12 +8101,16 @@
       <c r="M6">
         <v>4</v>
       </c>
-      <c r="N6">
-        <f t="shared" ref="N6:N13" si="4">ABS(L6-M6)</f>
+      <c r="N6" s="2">
+        <f>(M6-M5)/M5</f>
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O12" si="4">ABS(L6-M6)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8435,12 +8153,16 @@
       <c r="M7">
         <v>7</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N19" si="5">(M7-M6)/M6</f>
+        <v>0.75</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8483,12 +8205,16 @@
       <c r="M8">
         <v>11</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
+        <f t="shared" si="5"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8531,12 +8257,16 @@
       <c r="M9">
         <v>18</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="2">
+        <f t="shared" si="5"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8579,12 +8309,16 @@
       <c r="M10">
         <v>25</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="2">
+        <f t="shared" si="5"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8627,12 +8361,16 @@
       <c r="M11">
         <v>34</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="2">
+        <f t="shared" si="5"/>
+        <v>0.36</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8675,12 +8413,16 @@
       <c r="M12">
         <v>46</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="2">
+        <f t="shared" si="5"/>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8721,14 +8463,18 @@
         <v>66</v>
       </c>
       <c r="M13">
-        <v>57</v>
-      </c>
-      <c r="N13">
+        <v>59</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="O13">
         <f>ABS(L13-M13)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8750,11 +8496,37 @@
       <c r="G14">
         <v>55110</v>
       </c>
+      <c r="H14">
+        <v>2915</v>
+      </c>
       <c r="I14">
         <v>3703</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>788</v>
+      </c>
+      <c r="K14">
+        <f>ABS(H14-D14)</f>
+        <v>1941.3260006104701</v>
+      </c>
+      <c r="L14">
+        <f>ROUND(D14*0.0179799,0)</f>
+        <v>87</v>
+      </c>
+      <c r="M14">
+        <v>77</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="5"/>
+        <v>0.30508474576271188</v>
+      </c>
+      <c r="O14">
+        <f>ABS(L14-M14)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8776,8 +8548,30 @@
       <c r="G15">
         <v>55110</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>3417</v>
+      </c>
+      <c r="K15">
+        <f>ABS(H15-D15)</f>
+        <v>3000.9869511554198</v>
+      </c>
+      <c r="L15">
+        <f>ROUND(D15*0.0179799,0)</f>
+        <v>115</v>
+      </c>
+      <c r="M15">
+        <v>92</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="5"/>
+        <v>0.19480519480519481</v>
+      </c>
+      <c r="O15">
+        <f>ABS(L15-M15)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8799,16 +8593,30 @@
       <c r="G16">
         <v>55110</v>
       </c>
-      <c r="J16">
-        <f>AVERAGE(J3:J13)</f>
-        <v>140.54545454545453</v>
+      <c r="H16">
+        <v>3904</v>
       </c>
       <c r="K16">
-        <f>AVERAGE(K3:K13)</f>
-        <v>199.23659737577046</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <f>ABS(H16-D16)</f>
+        <v>4540.4458160399099</v>
+      </c>
+      <c r="L16">
+        <f>ROUND(D16*0.0179799,0)</f>
+        <v>152</v>
+      </c>
+      <c r="M16">
+        <v>114</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="5"/>
+        <v>0.2391304347826087</v>
+      </c>
+      <c r="O16">
+        <f>ABS(L16-M16)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8830,8 +8638,30 @@
       <c r="G17">
         <v>55110</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>4256</v>
+      </c>
+      <c r="K17">
+        <f>ABS(H17-D17)</f>
+        <v>6791.2873199641999</v>
+      </c>
+      <c r="L17">
+        <f>ROUND(D17*0.0179799,0)</f>
+        <v>199</v>
+      </c>
+      <c r="M17">
+        <v>136</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="5"/>
+        <v>0.19298245614035087</v>
+      </c>
+      <c r="O17">
+        <f>ABS(L17-M17)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8853,8 +8683,34 @@
       <c r="G18">
         <v>55110</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>4579</v>
+      </c>
+      <c r="J18">
+        <f>AVERAGE(J3:J14)</f>
+        <v>194.5</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE(K3:K16)</f>
+        <v>833.88295278137673</v>
+      </c>
+      <c r="L18">
+        <f>ROUND(D18*0.0179799,0)</f>
+        <v>258</v>
+      </c>
+      <c r="M18">
+        <v>159</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="5"/>
+        <v>0.16911764705882354</v>
+      </c>
+      <c r="O18">
+        <f>ABS(L18-M18)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8876,8 +8732,18 @@
       <c r="G19">
         <v>55110</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>5717</v>
+      </c>
+      <c r="M19">
+        <v>201</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="5"/>
+        <v>0.26415094339622641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8900,7 +8766,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8923,7 +8789,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8946,7 +8812,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8969,7 +8835,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8992,7 +8858,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9015,7 +8881,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9038,7 +8904,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9061,7 +8927,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9084,7 +8950,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9107,7 +8973,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9130,7 +8996,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9153,7 +9019,7 @@
         <v>55110</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>